<commit_message>
created DTY Edit bulk order script
</commit_message>
<xml_diff>
--- a/KatalonProjects/orderCreationData.xlsx
+++ b/KatalonProjects/orderCreationData.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="249"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="249" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DTYEdit" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>orderType</t>
   </si>
@@ -52,6 +53,9 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>showOrder</t>
   </si>
 </sst>
 </file>
@@ -496,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -594,4 +598,39 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>